<commit_message>
mlp job predictor major update
</commit_message>
<xml_diff>
--- a/msff/xls/job_satisfaction_predictor.xlsx
+++ b/msff/xls/job_satisfaction_predictor.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0x\repo1\msff\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\repos\repo1\msff\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD1D897-037F-4AD5-A4C6-D24850516102}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="-120" windowWidth="28560" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="-120" windowWidth="28560" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +19,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>HP</author>
   </authors>
   <commentList>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="121">
   <si>
     <t>GS</t>
   </si>
@@ -308,9 +307,6 @@
     <t>10 [d,e]</t>
   </si>
   <si>
-    <t>4 #low expectation</t>
-  </si>
-  <si>
     <t>3 #bonus</t>
   </si>
   <si>
@@ -393,9 +389,6 @@
     <t>1 #py,devops</t>
   </si>
   <si>
-    <t>3 #pric`</t>
-  </si>
-  <si>
     <t>4 #exec</t>
   </si>
   <si>
@@ -404,12 +397,38 @@
   <si>
     <t>$$$ $</t>
   </si>
+  <si>
+    <t>3 → 4 #low expectation</t>
+  </si>
+  <si>
+    <t>4++ #5M short</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">$$$ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>$$$</t>
+    </r>
+  </si>
+  <si>
+    <t>4++</t>
+  </si>
+  <si>
+    <t>4 #pric`</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -493,6 +512,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -914,23 +939,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -966,23 +974,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1158,12 +1149,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1003"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1362,7 +1353,7 @@
         <v>48</v>
       </c>
       <c r="O4" s="47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -1380,10 +1371,10 @@
     <row r="5" spans="1:27" ht="49.5">
       <c r="A5" s="1"/>
       <c r="B5" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="D5" s="5">
         <v>3</v>
@@ -1395,10 +1386,10 @@
         <v>75</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>31</v>
@@ -1437,7 +1428,7 @@
     <row r="6" spans="1:27" ht="16.5" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>59</v>
@@ -1470,7 +1461,7 @@
         <v>5</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>44</v>
@@ -1494,7 +1485,7 @@
     <row r="7" spans="1:27" ht="16.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="57">
         <v>2</v>
@@ -1547,7 +1538,7 @@
     <row r="8" spans="1:27" ht="16.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" s="19">
         <v>5</v>
@@ -1579,8 +1570,8 @@
       <c r="L8" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="M8" s="6">
-        <v>5</v>
+      <c r="M8" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>44</v>
@@ -1604,10 +1595,10 @@
     <row r="9" spans="1:27" ht="16.5" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>12</v>
@@ -1634,10 +1625,10 @@
         <v>13</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>44</v>
@@ -1676,7 +1667,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H10" s="4">
         <v>1</v>
@@ -1718,7 +1709,7 @@
     <row r="11" spans="1:27" ht="16.5" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="19">
         <v>5</v>
@@ -1771,7 +1762,7 @@
     <row r="12" spans="1:27" ht="16.5">
       <c r="A12" s="1"/>
       <c r="B12" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>85</v>
@@ -1824,7 +1815,7 @@
     <row r="13" spans="1:27" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A13" s="26"/>
       <c r="B13" s="45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>80</v>
@@ -1877,10 +1868,10 @@
     <row r="14" spans="1:27" ht="16.5" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="4">
         <v>3</v>
@@ -1892,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" s="4">
         <v>3</v>
@@ -1900,17 +1891,17 @@
       <c r="I14" s="4">
         <v>2</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>114</v>
+      <c r="J14" s="19" t="s">
+        <v>120</v>
       </c>
-      <c r="K14" s="4">
-        <v>4</v>
+      <c r="K14" s="19" t="s">
+        <v>119</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>33</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1930,7 +1921,7 @@
     <row r="15" spans="1:27" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A15" s="26"/>
       <c r="B15" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="28">
         <v>3</v>
@@ -1983,7 +1974,7 @@
     <row r="16" spans="1:27" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="31"/>
       <c r="B16" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="33">
         <v>2</v>
@@ -2065,7 +2056,7 @@
     <row r="18" spans="1:27" ht="33">
       <c r="A18" s="1"/>
       <c r="B18" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="58">
         <v>3</v>
@@ -2167,7 +2158,7 @@
     <row r="20" spans="1:27" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A20" s="31"/>
       <c r="B20" s="44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="36">
         <v>5</v>
@@ -2247,7 +2238,7 @@
     <row r="22" spans="1:27" s="29" customFormat="1" ht="16.5">
       <c r="A22" s="26"/>
       <c r="B22" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" s="59" t="s">
         <v>21</v>
@@ -2393,7 +2384,7 @@
     <row r="26" spans="1:27" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A26" s="26"/>
       <c r="B26" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -2610,7 +2601,7 @@
     <row r="33" spans="1:27" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A33" s="26"/>
       <c r="B33" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>
@@ -2641,7 +2632,7 @@
     <row r="34" spans="1:27" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A34" s="26"/>
       <c r="B34" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C34" s="38"/>
       <c r="D34" s="38"/>
@@ -2701,7 +2692,7 @@
     <row r="36" spans="1:27" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A36" s="26"/>
       <c r="B36" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" s="38"/>
       <c r="D36" s="38"/>
@@ -2762,13 +2753,13 @@
     </row>
     <row r="38" spans="1:27" ht="15" customHeight="1">
       <c r="B38" s="61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:27" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A39" s="26"/>
       <c r="B39" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" s="38"/>
       <c r="D39" s="38"/>
@@ -2799,7 +2790,7 @@
     <row r="40" spans="1:27" s="29" customFormat="1" ht="16.5" customHeight="1">
       <c r="A40" s="26"/>
       <c r="B40" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C40" s="38"/>
       <c r="D40" s="38"/>

</xml_diff>